<commit_message>
update ngày 13 tháng 12 + Thêm changPassword
</commit_message>
<xml_diff>
--- a/HAGAKI/HAGAKI/Resources/Productivity.xlsx
+++ b/HAGAKI/HAGAKI/Resources/Productivity.xlsx
@@ -86,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -111,28 +111,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -148,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -169,12 +147,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -541,7 +513,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -559,13 +531,13 @@
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="9"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="1:8" s="1" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">

</xml_diff>